<commit_message>
Adittional RF GS Results
</commit_message>
<xml_diff>
--- a/Analysis/RandomForest/May/24052023/summary_stats.xlsx
+++ b/Analysis/RandomForest/May/24052023/summary_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrismbrooks/Documents/Imperial/Asquith Group/KIR_HLA/Analysis/RandomForest/May/24052023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA73517-97DB-5A4F-897B-43126E796977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8EB300-EB07-B847-8250-94BE9BD09EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18080" yWindow="500" windowWidth="17480" windowHeight="20200" xr2:uid="{5316E3E2-5C85-E64C-9DE1-9B1C88E3518E}"/>
+    <workbookView xWindow="5260" yWindow="500" windowWidth="30300" windowHeight="19400" xr2:uid="{5316E3E2-5C85-E64C-9DE1-9B1C88E3518E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,10 +272,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$20</c:f>
+              <c:f>Sheet1!$C$8:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>25</c:v>
                 </c:pt>
@@ -307,23 +307,20 @@
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>250</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$8:$E$20</c:f>
+              <c:f>Sheet1!$E$8:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>-0.21041500985021899</c:v>
                 </c:pt>
@@ -367,6 +364,127 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CC78-584D-A830-6C53903E8F3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$8:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-0.21517390750568</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.210946066146663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.20914508083939401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.20868442297512199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.209773651757343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20909657813559299</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.211389560634346</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20913659799325399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.211561155206268</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.21237210884833199</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.211755813977624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CC78-584D-A830-6C53903E8F3D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2202,7 +2320,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2528,10 +2646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E9A1D7-D0A0-124C-BC92-DEB1BD0BF39B}">
-  <dimension ref="B7:E33"/>
+  <dimension ref="B7:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2557,7 +2675,9 @@
       <c r="C8" s="1">
         <v>25</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>-0.21517390750568</v>
+      </c>
       <c r="E8" s="1">
         <v>-0.21041500985021899</v>
       </c>
@@ -2569,7 +2689,9 @@
       <c r="C9" s="1">
         <v>50</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>-0.210946066146663</v>
+      </c>
       <c r="E9" s="1">
         <v>-0.21025087410593099</v>
       </c>
@@ -2581,7 +2703,9 @@
       <c r="C10" s="1">
         <v>75</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>-0.20914508083939401</v>
+      </c>
       <c r="E10" s="1">
         <v>-0.20534060199429399</v>
       </c>
@@ -2593,7 +2717,9 @@
       <c r="C11" s="1">
         <v>100</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>-0.20868442297512199</v>
+      </c>
       <c r="E11" s="1">
         <v>-0.20608251883874701</v>
       </c>
@@ -2605,7 +2731,9 @@
       <c r="C12" s="1">
         <v>125</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1">
+        <v>-0.209773651757343</v>
+      </c>
       <c r="E12" s="1">
         <v>-0.206807124114158</v>
       </c>
@@ -2617,7 +2745,9 @@
       <c r="C13" s="1">
         <v>150</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <v>-0.20909657813559299</v>
+      </c>
       <c r="E13" s="1">
         <v>-0.20710521882821001</v>
       </c>
@@ -2629,7 +2759,9 @@
       <c r="C14" s="1">
         <v>175</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1">
+        <v>-0.211389560634346</v>
+      </c>
       <c r="E14" s="1">
         <v>-0.21041565147027</v>
       </c>
@@ -2641,7 +2773,9 @@
       <c r="C15" s="1">
         <v>200</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1">
+        <v>-0.20913659799325399</v>
+      </c>
       <c r="E15" s="1">
         <v>-0.209935731961954</v>
       </c>
@@ -2653,7 +2787,9 @@
       <c r="C16" s="1">
         <v>225</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1">
+        <v>-0.211561155206268</v>
+      </c>
       <c r="E16" s="1">
         <v>-0.208269124999403</v>
       </c>
@@ -2665,19 +2801,23 @@
       <c r="C17" s="1">
         <v>250</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <v>-0.21237210884833199</v>
+      </c>
       <c r="E17" s="1">
         <v>-0.20366230211026401</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>7</v>
       </c>
-      <c r="C18" s="4">
-        <v>250</v>
-      </c>
-      <c r="D18" s="5"/>
+      <c r="C18" s="1">
+        <v>275</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-0.211755813977624</v>
+      </c>
       <c r="E18" s="1">
         <v>-0.20956921633554601</v>
       </c>
@@ -2843,18 +2983,47 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="1">
+      <c r="B33" s="4">
         <v>9</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="4">
         <v>250</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="4">
         <v>-0.208285390594313</v>
       </c>
       <c r="E33">
         <v>-0.20720125553323901</v>
       </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="4">
+        <v>9</v>
+      </c>
+      <c r="C34" s="4">
+        <v>275</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="5">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1">
+        <v>500</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="5">
+        <v>9</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>